<commit_message>
New Test results for sha2-384 and sha2-512
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moritz Joekel\source\repos\CredentialLeakageMonitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85769E66-5239-4AF4-A680-A90CD4C3CAD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BE125A-F2A7-452A-97B4-132D7F72D5B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A97F8195-80A5-4440-B254-68AAA14C9DA5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A97F8195-80A5-4440-B254-68AAA14C9DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Verfahren</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>AES_256</t>
+  </si>
+  <si>
+    <t>SHA_384</t>
   </si>
 </sst>
 </file>
@@ -498,27 +501,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112916B0-1CBF-4C5B-BC7A-523B0D2A6D77}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="19" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="27.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="23.88671875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="23.44140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="23.109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="32.44140625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="29.88671875" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="32.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -556,7 +559,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -593,7 +596,7 @@
         <v>1847.3333333333333</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -630,7 +633,7 @@
         <v>1863.6666666666667</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -638,20 +641,20 @@
         <v>100000</v>
       </c>
       <c r="C4" s="2">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2">
-        <v>1649</v>
+        <v>2005</v>
       </c>
       <c r="E4" s="2">
-        <v>1683</v>
+        <v>1809</v>
       </c>
       <c r="F4" s="2">
-        <v>1073</v>
+        <v>1566</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" si="0"/>
-        <v>1468.3333333333333</v>
+        <v>1793.3333333333333</v>
       </c>
       <c r="H4" s="2">
         <v>1992</v>
@@ -667,44 +670,44 @@
         <v>1743</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B5" s="1">
         <v>100000</v>
       </c>
       <c r="C5" s="2">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2">
-        <v>1504</v>
+        <v>1758</v>
       </c>
       <c r="E5" s="2">
-        <v>1494</v>
+        <v>1524</v>
       </c>
       <c r="F5" s="2">
-        <v>1089</v>
+        <v>1139</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>1362.3333333333333</v>
+        <v>1473.6666666666667</v>
       </c>
       <c r="H5" s="2">
-        <v>2156</v>
+        <v>1127</v>
       </c>
       <c r="I5" s="2">
-        <v>1348</v>
+        <v>945</v>
       </c>
       <c r="J5" s="2">
-        <v>1389</v>
+        <v>997</v>
       </c>
       <c r="K5" s="2">
         <f t="shared" si="1"/>
-        <v>1631</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -744,7 +747,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -784,12 +787,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -826,7 +829,7 @@
         <v>271521</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Test results except AES_256
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moritz Joekel\source\repos\CredentialLeakageMonitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27444813-89FB-4A5D-BB0E-4B7A26423491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2171E912-1117-4701-8335-3093FCE7C537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A97F8195-80A5-4440-B254-68AAA14C9DA5}"/>
   </bookViews>
@@ -501,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112916B0-1CBF-4C5B-BC7A-523B0D2A6D77}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,13 +714,34 @@
       <c r="B6" s="1">
         <v>100000</v>
       </c>
-      <c r="G6" s="2" t="e">
+      <c r="C6" s="2">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2">
+        <v>285773</v>
+      </c>
+      <c r="E6" s="2">
+        <v>258742</v>
+      </c>
+      <c r="F6" s="2">
+        <v>252924</v>
+      </c>
+      <c r="G6" s="2">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K6" s="2" t="e">
+        <v>265813</v>
+      </c>
+      <c r="H6" s="2">
+        <v>300256</v>
+      </c>
+      <c r="I6" s="2">
+        <v>291567</v>
+      </c>
+      <c r="J6" s="2">
+        <v>289534</v>
+      </c>
+      <c r="K6" s="2">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>293785.66666666669</v>
       </c>
       <c r="L6" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Test results 1mio SHA3_512
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moritz Joekel\source\repos\CredentialLeakageMonitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FFFD1E-B742-47CC-A914-091F409A32BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B75B084-938A-4D79-806F-D78914575AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14505" yWindow="75" windowWidth="14610" windowHeight="15585" xr2:uid="{A97F8195-80A5-4440-B254-68AAA14C9DA5}"/>
+    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{A97F8195-80A5-4440-B254-68AAA14C9DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>Verfahren</t>
   </si>
@@ -494,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112916B0-1CBF-4C5B-BC7A-523B0D2A6D77}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,7 +615,7 @@
         <v>1510</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G15" si="0">AVERAGE(D3:F3)</f>
+        <f t="shared" ref="G3:G19" si="0">AVERAGE(D3:F3)</f>
         <v>1732.6666666666667</v>
       </c>
       <c r="H3" s="2">
@@ -669,7 +669,7 @@
         <v>875</v>
       </c>
       <c r="K4" s="2">
-        <f t="shared" ref="K4:K14" si="2">AVERAGE(H4:J4)</f>
+        <f t="shared" ref="K4:K18" si="2">AVERAGE(H4:J4)</f>
         <v>1135</v>
       </c>
       <c r="L4" s="7">
@@ -807,7 +807,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1">
         <v>1000000</v>
@@ -816,39 +816,39 @@
         <v>14</v>
       </c>
       <c r="D9" s="2">
-        <v>12831</v>
+        <v>9828</v>
       </c>
       <c r="E9" s="2">
-        <v>10174</v>
+        <v>10317</v>
       </c>
       <c r="F9" s="2">
-        <v>10178</v>
+        <v>9784</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v>11061</v>
+        <v>9976.3333333333339</v>
       </c>
       <c r="H9" s="2">
-        <v>10178</v>
+        <v>11752</v>
       </c>
       <c r="I9" s="2">
-        <v>11810</v>
+        <v>11436</v>
       </c>
       <c r="J9" s="2">
-        <v>11621</v>
+        <v>11257</v>
       </c>
       <c r="K9" s="2">
         <f t="shared" si="2"/>
-        <v>11203</v>
+        <v>11481.666666666666</v>
       </c>
       <c r="L9" s="7">
-        <f t="shared" ref="L9:L10" si="3">(K9*500)/1000/60/60</f>
-        <v>1.5559722222222223</v>
+        <f t="shared" ref="L9:L12" si="3">(K9*500)/1000/60/60</f>
+        <v>1.594675925925926</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1">
         <v>1000000</v>
@@ -856,198 +856,326 @@
       <c r="C10" s="2">
         <v>14</v>
       </c>
-      <c r="D10" s="2">
+      <c r="G10" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K10" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L10" s="7" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C11" s="2">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2">
+        <v>12831</v>
+      </c>
+      <c r="E11" s="2">
+        <v>10174</v>
+      </c>
+      <c r="F11" s="2">
+        <v>10178</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>11061</v>
+      </c>
+      <c r="H11" s="2">
+        <v>10178</v>
+      </c>
+      <c r="I11" s="2">
+        <v>11810</v>
+      </c>
+      <c r="J11" s="2">
+        <v>11621</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="2"/>
+        <v>11203</v>
+      </c>
+      <c r="L11" s="7">
+        <f t="shared" si="3"/>
+        <v>1.5559722222222223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="C12" s="2">
+        <v>14</v>
+      </c>
+      <c r="D12" s="2">
         <v>10440</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E12" s="2">
         <v>11770</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F12" s="2">
         <v>10308</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G12" s="2">
         <f t="shared" si="0"/>
         <v>10839.333333333334</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H12" s="2">
         <v>11174</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I12" s="2">
         <v>11643</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J12" s="2">
         <v>11730</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K12" s="2">
         <f t="shared" si="2"/>
         <v>11515.666666666666</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L12" s="7">
         <f t="shared" si="3"/>
         <v>1.5993981481481481</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B13" s="1">
         <v>1000000</v>
       </c>
-      <c r="C11" s="2">
-        <v>14</v>
-      </c>
-      <c r="D11" s="2">
+      <c r="C13" s="2">
+        <v>14</v>
+      </c>
+      <c r="D13" s="2">
         <v>9427</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E13" s="2">
         <v>9451</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F13" s="2">
         <v>9058</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G13" s="2">
         <f t="shared" si="0"/>
         <v>9312</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H13" s="2">
         <v>10312</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I13" s="2">
         <v>9041</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J13" s="2">
         <v>11012</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K13" s="2">
         <f t="shared" si="2"/>
         <v>10121.666666666666</v>
       </c>
-      <c r="L11" s="7">
-        <f>(K11*500)/1000/60/60</f>
+      <c r="L13" s="7">
+        <f>(K13*500)/1000/60/60</f>
         <v>1.4057870370370369</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2000000</v>
+      </c>
+      <c r="C15" s="2">
+        <v>14</v>
+      </c>
+      <c r="D15" s="2">
+        <v>19946</v>
+      </c>
+      <c r="E15" s="2">
+        <v>19402</v>
+      </c>
+      <c r="F15" s="2">
+        <v>20340</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>19896</v>
+      </c>
+      <c r="H15" s="2">
+        <v>21951</v>
+      </c>
+      <c r="I15" s="2">
+        <v>24499</v>
+      </c>
+      <c r="J15" s="2">
+        <v>24550</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="2"/>
+        <v>23666.666666666668</v>
+      </c>
+      <c r="L15" s="8">
+        <f t="shared" ref="L15:L18" si="4">(K15*250)/1000/60/60</f>
+        <v>1.6435185185185186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2000000</v>
+      </c>
+      <c r="C16" s="2">
+        <v>14</v>
+      </c>
+      <c r="G16" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K16" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L16" s="8" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B17" s="1">
         <v>2000000</v>
       </c>
-      <c r="C13" s="2">
-        <v>14</v>
-      </c>
-      <c r="D13" s="2">
+      <c r="C17" s="2">
+        <v>14</v>
+      </c>
+      <c r="D17" s="2">
         <v>17698</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E17" s="2">
         <v>17809</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F17" s="2">
         <v>19248</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G17" s="2">
         <f t="shared" si="0"/>
         <v>18251.666666666668</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H17" s="2">
         <v>22495</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I17" s="2">
         <v>21999</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J17" s="2">
         <v>22660</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K17" s="2">
         <f t="shared" si="2"/>
         <v>22384.666666666668</v>
       </c>
-      <c r="L13" s="8">
-        <f t="shared" ref="L13:L14" si="4">(K13*250)/1000/60/60</f>
+      <c r="L17" s="8">
+        <f t="shared" si="4"/>
         <v>1.5544907407407407</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B18" s="1">
         <v>2000000</v>
       </c>
-      <c r="C14" s="2">
-        <v>14</v>
-      </c>
-      <c r="D14" s="2">
+      <c r="C18" s="2">
+        <v>14</v>
+      </c>
+      <c r="D18" s="2">
         <v>18692</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E18" s="2">
         <v>18628</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F18" s="2">
         <v>18329</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G18" s="2">
         <f t="shared" si="0"/>
         <v>18549.666666666668</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H18" s="2">
         <v>23011</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I18" s="2">
         <v>21875</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J18" s="2">
         <v>24593</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K18" s="2">
         <f t="shared" si="2"/>
         <v>23159.666666666668</v>
       </c>
-      <c r="L14" s="8">
+      <c r="L18" s="8">
         <f t="shared" si="4"/>
         <v>1.6083101851851853</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B19" s="1">
         <v>2000000</v>
       </c>
-      <c r="C15" s="2">
-        <v>14</v>
-      </c>
-      <c r="D15" s="2">
+      <c r="C19" s="2">
+        <v>14</v>
+      </c>
+      <c r="D19" s="2">
         <v>18091</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E19" s="2">
         <v>17940</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F19" s="2">
         <v>19170</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G19" s="2">
         <f t="shared" si="0"/>
         <v>18400.333333333332</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H19" s="2">
         <v>19979</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I19" s="2">
         <v>21329</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J19" s="2">
         <v>24025</v>
       </c>
-      <c r="K15" s="2">
-        <f>AVERAGE(H15:J15)</f>
+      <c r="K19" s="2">
+        <f>AVERAGE(H19:J19)</f>
         <v>21777.666666666668</v>
       </c>
-      <c r="L15" s="8">
-        <f>(K15*250)/1000/60/60</f>
+      <c r="L19" s="8">
+        <f>(K19*250)/1000/60/60</f>
         <v>1.512337962962963</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Test Results SHA3_384 1-2mio
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moritz Joekel\source\repos\CredentialLeakageMonitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B75B084-938A-4D79-806F-D78914575AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D4A283-E965-4392-A00B-2163C1D9EB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{A97F8195-80A5-4440-B254-68AAA14C9DA5}"/>
+    <workbookView xWindow="-14505" yWindow="75" windowWidth="14610" windowHeight="15585" xr2:uid="{A97F8195-80A5-4440-B254-68AAA14C9DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -496,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112916B0-1CBF-4C5B-BC7A-523B0D2A6D77}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,17 +856,35 @@
       <c r="C10" s="2">
         <v>14</v>
       </c>
-      <c r="G10" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K10" s="2" t="e">
+      <c r="D10" s="2">
+        <v>10952</v>
+      </c>
+      <c r="E10" s="2">
+        <v>9042</v>
+      </c>
+      <c r="F10" s="2">
+        <v>9875</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>9956.3333333333339</v>
+      </c>
+      <c r="H10" s="2">
+        <v>10246</v>
+      </c>
+      <c r="I10" s="2">
+        <v>10249</v>
+      </c>
+      <c r="J10" s="2">
+        <v>10333</v>
+      </c>
+      <c r="K10" s="2">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L10" s="7" t="e">
+        <v>10276</v>
+      </c>
+      <c r="L10" s="7">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>1.4272222222222224</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1043,17 +1061,35 @@
       <c r="C16" s="2">
         <v>14</v>
       </c>
-      <c r="G16" s="2" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K16" s="2" t="e">
+      <c r="D16" s="2">
+        <v>19230</v>
+      </c>
+      <c r="E16" s="2">
+        <v>18670</v>
+      </c>
+      <c r="F16" s="2">
+        <v>18677</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>18859</v>
+      </c>
+      <c r="H16" s="2">
+        <v>21042</v>
+      </c>
+      <c r="I16" s="2">
+        <v>21777</v>
+      </c>
+      <c r="J16" s="2">
+        <v>23961</v>
+      </c>
+      <c r="K16" s="2">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L16" s="8" t="e">
+        <v>22260</v>
+      </c>
+      <c r="L16" s="8">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
+        <v>1.5458333333333334</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>